<commit_message>
Updated images and code examples
</commit_message>
<xml_diff>
--- a/Chapter 03/images/B12258_03_8_2.xlsx
+++ b/Chapter 03/images/B12258_03_8_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01 Bitbucket\Hands-On-Microservices-with-C-8-and-.NET-Core-3.0-Third-Edition\Chapter 03\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A47B1D-DE35-4426-8A5D-2EF321DF7492}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDED43C-6F1E-44A4-BF26-2F14B9918928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{97CD2F51-6D34-48C9-B032-DC92125CBCAC}"/>
   </bookViews>
@@ -35,9 +35,6 @@
     <t>GitHub</t>
   </si>
   <si>
-    <t>VSTS</t>
-  </si>
-  <si>
     <t>Azure Container Registery</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>(8)</t>
+  </si>
+  <si>
+    <t>Azure DevOps</t>
   </si>
 </sst>
 </file>
@@ -349,14 +349,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -364,22 +403,25 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -417,48 +459,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1212,7 +1212,7 @@
   <dimension ref="E3:S18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:S18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,316 +1220,318 @@
     <col min="1" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="7" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="27"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="6"/>
     </row>
     <row r="4" spans="5:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="30"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="22"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="9"/>
     </row>
     <row r="5" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="30"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="9"/>
     </row>
     <row r="6" spans="5:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="S6" s="30"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="9"/>
     </row>
     <row r="7" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="28"/>
-      <c r="F7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="23"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="30"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="37"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="9"/>
     </row>
     <row r="8" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E8" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="30"/>
+      <c r="E8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="28"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="9"/>
     </row>
     <row r="9" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E9" s="34"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="36" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="36" t="s">
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="N9" s="16"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="9"/>
     </row>
     <row r="10" spans="5:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="28"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="12" t="s">
+      <c r="G10" s="8"/>
+      <c r="H10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="30"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="19"/>
+      <c r="S10" s="9"/>
     </row>
     <row r="11" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="30"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="9"/>
     </row>
     <row r="12" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="30"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="9"/>
     </row>
     <row r="13" spans="5:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="30"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="9"/>
     </row>
     <row r="14" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="19"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="30"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="33"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="9"/>
     </row>
     <row r="15" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="30"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="9"/>
     </row>
     <row r="16" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="30"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="9"/>
     </row>
     <row r="17" spans="5:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17" s="3"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="30"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="9"/>
     </row>
     <row r="18" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="33"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>